<commit_message>
updated schematic, changed bom slightly
</commit_message>
<xml_diff>
--- a/AntiSpark BOM.xlsx
+++ b/AntiSpark BOM.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthew\Documents\GitHub\Anti-Spark_Switch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\GitHub\Anti-Spark_Switch\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7099B27F-4406-4714-8119-52B8E9CB20F3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10910"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Turnkey" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Turnkey!$A$1:$K$10</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Turnkey!$A$1:$K$11</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
   <si>
     <t>Description</t>
   </si>
@@ -208,12 +209,21 @@
   </si>
   <si>
     <t>581-06033C105KAT2A</t>
+  </si>
+  <si>
+    <t>R4,R5</t>
+  </si>
+  <si>
+    <t>16.5K Resistor</t>
+  </si>
+  <si>
+    <t>1206</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
@@ -730,31 +740,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R27"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.7265625" customWidth="1"/>
-    <col min="2" max="2" width="4.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="85.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.54296875" customWidth="1"/>
-    <col min="8" max="8" width="13.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.1796875" customWidth="1"/>
-    <col min="10" max="10" width="14.26953125" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>23</v>
       </c>
@@ -767,7 +777,7 @@
       <c r="H1" s="31"/>
       <c r="I1" s="31"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -775,7 +785,7 @@
       <c r="G2" s="1"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>3</v>
       </c>
@@ -816,7 +826,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="24"/>
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
@@ -829,12 +839,12 @@
       <c r="J5" s="27"/>
       <c r="K5" s="27"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="23">
         <v>1</v>
       </c>
       <c r="B6" s="16">
-        <f>(3*G14)</f>
+        <f>(3*G15)</f>
         <v>3</v>
       </c>
       <c r="C6" s="16" t="s">
@@ -870,12 +880,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="23">
         <v>2</v>
       </c>
       <c r="B7" s="14">
-        <f>(2*G14)</f>
+        <f>(2*G15)</f>
         <v>2</v>
       </c>
       <c r="C7" s="16" t="s">
@@ -895,7 +905,7 @@
         <v>0.15</v>
       </c>
       <c r="H7" s="18">
-        <f t="shared" ref="H7:H12" si="0">(B7*G7)</f>
+        <f t="shared" ref="H7:H13" si="0">(B7*G7)</f>
         <v>0.3</v>
       </c>
       <c r="I7" s="16" t="s">
@@ -911,12 +921,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="23">
         <v>3</v>
       </c>
       <c r="B8" s="14">
-        <f>(1*G14)</f>
+        <f>(1*G15)</f>
         <v>1</v>
       </c>
       <c r="C8" s="16" t="s">
@@ -949,210 +959,242 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="23">
         <v>4</v>
       </c>
       <c r="B9" s="14">
-        <f>(1*G14)</f>
-        <v>1</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>61</v>
-      </c>
+        <f>(2*G15)</f>
+        <v>2</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="17"/>
       <c r="G9" s="18">
-        <f>IF(B9&lt;=49,0.11,IF(B9&lt;=99,0.109,IF(B9&lt;=499,0.106)))</f>
-        <v>0.11</v>
+        <f>IF(B9&lt;=9,0.15,IF(B9&lt;=99,0.014,IF(B9&lt;=999,0.006)))</f>
+        <v>0.15</v>
       </c>
       <c r="H9" s="18">
-        <f>(B9*G9)</f>
-        <v>0.11</v>
+        <f t="shared" si="0"/>
+        <v>0.3</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="J9" s="20" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="K9" s="16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="23">
         <v>5</v>
       </c>
       <c r="B10" s="14">
-        <f>(1*G14)</f>
+        <f>(1*G15)</f>
         <v>1</v>
       </c>
       <c r="C10" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="18">
+        <f>IF(B10&lt;=49,0.11,IF(B10&lt;=99,0.109,IF(B10&lt;=499,0.106)))</f>
+        <v>0.11</v>
+      </c>
+      <c r="H10" s="18">
+        <f>(B10*G10)</f>
+        <v>0.11</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="23">
+        <v>6</v>
+      </c>
+      <c r="B11" s="14">
+        <f>(1*G15)</f>
+        <v>1</v>
+      </c>
+      <c r="C11" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D11" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E11" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F11" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="18">
-        <f>IF(B10&lt;=24,0.15,IF(B10&lt;=99,0.013,IF(B10&lt;=249,0.073)))</f>
+      <c r="G11" s="18">
+        <f>IF(B11&lt;=24,0.15,IF(B11&lt;=99,0.013,IF(B11&lt;=249,0.073)))</f>
         <v>0.15</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H11" s="18">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="I10" s="16" t="s">
+      <c r="I11" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="J11" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="K10" s="16" t="s">
+      <c r="K11" s="16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="23">
-        <v>5</v>
-      </c>
-      <c r="B11" s="14">
-        <f>(2*G14)</f>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" s="23">
+        <v>7</v>
+      </c>
+      <c r="B12" s="14">
+        <f>(2*G15)</f>
         <v>2</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C12" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D12" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E12" s="14">
         <v>7460408</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F12" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="18">
-        <f>IF(B10&lt;=9,3.89,IF(B10&lt;=49,3.6,IF(B10&lt;=99,3.27)))</f>
+      <c r="G12" s="18">
+        <f>IF(B11&lt;=9,3.89,IF(B11&lt;=49,3.6,IF(B11&lt;=99,3.273)))</f>
         <v>3.89</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H12" s="18">
         <f t="shared" si="0"/>
         <v>7.78</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="I12" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="J12" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="K11" s="16" t="s">
+      <c r="K12" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="23">
-        <v>5</v>
-      </c>
-      <c r="B12" s="14">
-        <f>(1*G14)</f>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="23">
+        <v>8</v>
+      </c>
+      <c r="B13" s="14">
+        <f>(1*G15)</f>
         <v>1</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C13" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D13" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E13" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F13" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="18">
-        <f>IF(B12&lt;=9,7.25,IF(B12&lt;=24,6,IF(B12&lt;=49,5.76)))</f>
-        <v>7.25</v>
-      </c>
-      <c r="H12" s="18">
+      <c r="G13" s="18">
+        <f>IF(B13&lt;=4,3.3,IF(B13&lt;=9,3.19,IF(B13&lt;=49,3.08)))</f>
+        <v>3.3</v>
+      </c>
+      <c r="H13" s="18">
         <f t="shared" si="0"/>
-        <v>7.25</v>
-      </c>
-      <c r="I12" s="16" t="s">
+        <v>3.3</v>
+      </c>
+      <c r="I13" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="J12" s="16" t="s">
+      <c r="J13" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="K12" s="16" t="s">
+      <c r="K13" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="I13" s="12"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F14" s="28" t="s">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I14" s="12"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F15" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G15" s="1">
         <v>1</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="H15" s="9">
-        <f>SUM(H6:H12)</f>
-        <v>26.69</v>
-      </c>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="H16" s="1"/>
-      <c r="I16" s="6"/>
-    </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H17" s="7"/>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H18" s="9"/>
-    </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H20" s="7" t="s">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="H16" s="9">
+        <f>(SUM(H6:H13)) / G15</f>
+        <v>23.040000000000003</v>
+      </c>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="H17" s="1"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="H18" s="7"/>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="H19" s="9"/>
+    </row>
+    <row r="21" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="H21" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H21" s="9">
-        <f>SUM(H15+H18)</f>
-        <v>26.69</v>
-      </c>
-    </row>
-    <row r="27" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H27" s="11"/>
+    <row r="22" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="H22" s="9">
+        <f>SUM(H16+H19)</f>
+        <v>23.040000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="H28" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>